<commit_message>
Update floorplan, schedules, and details
</commit_message>
<xml_diff>
--- a/smrt_Elec/panel/PNL_A.xlsx
+++ b/smrt_Elec/panel/PNL_A.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\classes\sust\smrt_Elec\panel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B00FE5-7CAB-4C69-AA7A-DF98CC80826F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,61 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+  <si>
+    <t>15A</t>
+  </si>
+  <si>
+    <t>*INSTALL GFCI BREAKER</t>
+  </si>
+  <si>
+    <t>OUTDOOR RECEPTACLES*</t>
+  </si>
+  <si>
+    <t>BATHROOM RECEPTACLES*</t>
+  </si>
+  <si>
+    <t>LIGHTING</t>
+  </si>
+  <si>
+    <t>LIVING SPACE RECEPTACLES</t>
+  </si>
+  <si>
+    <t>BASEBOARD HEATER</t>
+  </si>
+  <si>
+    <t>RWH PUMP</t>
+  </si>
+  <si>
+    <t>CCT</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>RATING</t>
+  </si>
+  <si>
+    <t>PANEL A</t>
+  </si>
+  <si>
+    <t>1 Ø, 2W</t>
+  </si>
+  <si>
+    <t>MAIN BREAKER:</t>
+  </si>
+  <si>
+    <t>60A</t>
+  </si>
+  <si>
+    <t>PHASE, WIRE</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -45,12 +104,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +499,312 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="8"/>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="13">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>2</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="13">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>3</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="13">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>